<commit_message>
[FIX] lot of fixes after refactoring
</commit_message>
<xml_diff>
--- a/goufi_base/tests/data/xlsx/testing.xlsx
+++ b/goufi_base/tests/data/xlsx/testing.xlsx
@@ -66,6 +66,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,32 +148,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A4:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -195,14 +193,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,7 +236,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -260,13 +256,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>